<commit_message>
wells added now properly
</commit_message>
<xml_diff>
--- a/Assignments/Week 3 - ATES/GIS/new_wells.xlsx
+++ b/Assignments/Week 3 - ATES/GIS/new_wells.xlsx
@@ -10,12 +10,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>fid</t>
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
   <si>
     <t>Koud</t>
@@ -80,6 +86,8 @@
   <cols>
     <col min="1" max="1024" width="15"/>
     <col min="2" max="1024" width="15"/>
+    <col min="3" max="1024" width="15"/>
+    <col min="4" max="1024" width="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -89,13 +97,25 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>96602</v>
+      </c>
+      <c r="D2">
+        <v>437272</v>
       </c>
     </row>
     <row r="3">
@@ -103,7 +123,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>96588</v>
+      </c>
+      <c r="D3">
+        <v>437350</v>
       </c>
     </row>
     <row r="4">
@@ -111,7 +137,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>96668</v>
+      </c>
+      <c r="D4">
+        <v>437322</v>
       </c>
     </row>
     <row r="5">
@@ -119,44 +151,69 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>96527</v>
+      </c>
+      <c r="D5">
+        <v>437289</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>96776</v>
+      </c>
+      <c r="D6">
+        <v>437219</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>96840</v>
+      </c>
+      <c r="D7">
+        <v>437279</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>96870</v>
+      </c>
+      <c r="D8">
+        <v>437196</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>96927</v>
+      </c>
+      <c r="D9">
+        <v>437260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>